<commit_message>
fifth commit, kazakh language and refactoring
</commit_message>
<xml_diff>
--- a/output_file.xlsx
+++ b/output_file.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,7 +466,7 @@
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45118.42943287037</v>
+        <v>45124.76650462963</v>
       </c>
     </row>
     <row r="3">
@@ -477,11 +477,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>База знаний</t>
+          <t>/start</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45118.42943287037</v>
+        <v>45124.76678240741</v>
       </c>
     </row>
     <row r="4">
@@ -492,11 +492,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>База инструкций</t>
+          <t>/start</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45118.42943287037</v>
+        <v>45124.7668287037</v>
       </c>
     </row>
     <row r="5">
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>45118.4312037037</v>
+        <v>45124.77592592593</v>
       </c>
     </row>
     <row r="6">
@@ -522,11 +522,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>База знаний</t>
+          <t>/start</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>45118.4312037037</v>
+        <v>45124.77693287037</v>
       </c>
     </row>
     <row r="7">
@@ -537,11 +537,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>База инструкций</t>
+          <t>/start</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>45118.4312037037</v>
+        <v>45124.77695601852</v>
       </c>
     </row>
     <row r="8">
@@ -552,11 +552,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>/start</t>
+          <t>База знаний</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>45118.4312037037</v>
+        <v>45124.77998842593</v>
       </c>
     </row>
     <row r="9">
@@ -567,11 +567,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>База знаний</t>
+          <t>База инструкций</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>45118.4312037037</v>
+        <v>45124.78003472222</v>
       </c>
     </row>
     <row r="10">
@@ -582,11 +582,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>База инструкций</t>
+          <t>Lotus | Инструкции</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>45118.4312037037</v>
+        <v>45124.7800462963</v>
       </c>
     </row>
     <row r="11">
@@ -597,11 +597,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>/start</t>
+          <t>portal.telecom.kz | Инструкции</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>45118.43591435185</v>
+        <v>45124.78006944444</v>
       </c>
     </row>
     <row r="12">
@@ -612,11 +612,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>База знаний</t>
+          <t>menu</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>45118.43591435185</v>
+        <v>45124.78025462963</v>
       </c>
     </row>
     <row r="13">
@@ -627,11 +627,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>База инструкций</t>
+          <t>База знаний</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>45118.43591435185</v>
+        <v>45124.78034722222</v>
       </c>
     </row>
     <row r="14">
@@ -642,71 +642,71 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>/start</t>
+          <t>Глоссарий</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>45118.43805555555</v>
+        <v>45124.78037037037</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>760906879</t>
+          <t>484489968</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>База знаний</t>
+          <t>/start</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>45118.43805555555</v>
+        <v>45124.78109953704</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>760906879</t>
+          <t>484489968</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>База инструкций</t>
+          <t>/start</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>45118.43805555555</v>
+        <v>45124.78113425926</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>760906879</t>
+          <t>484489968</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>/start</t>
+          <t>Білім базасы</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>45118.44072916666</v>
+        <v>45124.78116898148</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>760906879</t>
+          <t>484489968</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>База знаний</t>
+          <t>Нұсқаулық базасы</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
-        <v>45118.44072916666</v>
+        <v>45124.78119212963</v>
       </c>
     </row>
     <row r="19">
@@ -717,11 +717,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>База инструкций</t>
+          <t>menu</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>45118.44072916666</v>
+        <v>45124.78180555555</v>
       </c>
     </row>
     <row r="20">
@@ -732,11 +732,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>portal.telecom.kz | Инструкции</t>
+          <t>База знаний</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>45118.44072916666</v>
+        <v>45124.7818287037</v>
       </c>
     </row>
     <row r="21">
@@ -747,11 +747,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>/start</t>
+          <t>База инструкций</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
-        <v>45118.44072916666</v>
+        <v>45124.78184027778</v>
       </c>
     </row>
     <row r="22">
@@ -762,11 +762,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Welcome курс | Адаптация</t>
+          <t>CheckPoint VPN | Удаленная работа</t>
         </is>
       </c>
       <c r="C22" s="2" t="n">
-        <v>45118.44072916666</v>
+        <v>45124.78186342592</v>
       </c>
     </row>
     <row r="23">
@@ -777,11 +777,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Рассказывай!</t>
+          <t>Логотипы и Брендбук</t>
         </is>
       </c>
       <c r="C23" s="2" t="n">
-        <v>45118.44072916666</v>
+        <v>45124.78188657408</v>
       </c>
     </row>
     <row r="24">
@@ -792,11 +792,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>menu</t>
+          <t>Личный кабинет telecom.kz</t>
         </is>
       </c>
       <c r="C24" s="2" t="n">
-        <v>45118.44072916666</v>
+        <v>45124.78190972222</v>
       </c>
     </row>
     <row r="25">
@@ -807,11 +807,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Оставить обращение</t>
+          <t>Модемы | Настройка</t>
         </is>
       </c>
       <c r="C25" s="2" t="n">
-        <v>45118.44072916666</v>
+        <v>45124.78192129629</v>
       </c>
     </row>
     <row r="26">
@@ -822,11 +822,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Обучение | Корпоративный Университет</t>
+          <t>Lotus | Инструкции</t>
         </is>
       </c>
       <c r="C26" s="2" t="n">
-        <v>45118.44072916666</v>
+        <v>45124.78193287037</v>
       </c>
     </row>
     <row r="27">
@@ -837,11 +837,11 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Служба поддержки “Нысана"</t>
+          <t>portal.telecom.kz | Инструкции</t>
         </is>
       </c>
       <c r="C27" s="2" t="n">
-        <v>45118.44072916666</v>
+        <v>45124.78197916667</v>
       </c>
     </row>
     <row r="28">
@@ -856,7 +856,7 @@
         </is>
       </c>
       <c r="C28" s="2" t="n">
-        <v>45118.44072916666</v>
+        <v>45124.7893287037</v>
       </c>
     </row>
     <row r="29">
@@ -867,11 +867,1601 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>База знаний</t>
+          <t>Welcome курс | Адаптация</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
-        <v>45118.44072916666</v>
+        <v>45124.789375</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Рассказывай!</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>45124.78942129629</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Рассказывай!</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>45124.78946759259</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>45124.78996527778</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Заполнить карточку БиОТ</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>45124.79002314815</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Опасный фактор/условие</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>45124.79004629629</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C35" s="2" t="n">
+        <v>45124.79011574074</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Часто задаваемые вопросы</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>45124.79015046296</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Демеу</t>
+        </is>
+      </c>
+      <c r="C37" s="2" t="n">
+        <v>45124.79017361111</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C38" s="2" t="n">
+        <v>45124.79027777778</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Часто задаваемые вопросы</t>
+        </is>
+      </c>
+      <c r="C39" s="2" t="n">
+        <v>45124.7903125</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Вопросы к HR</t>
+        </is>
+      </c>
+      <c r="C40" s="2" t="n">
+        <v>45124.79032407407</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="C41" s="2" t="n">
+        <v>45124.88746527778</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="C42" s="2" t="n">
+        <v>45124.88791666667</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C43" s="2" t="n">
+        <v>45124.88811342593</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C44" s="2" t="n">
+        <v>45124.88859953704</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C45" s="2" t="n">
+        <v>45124.88899305555</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C46" s="2" t="n">
+        <v>45124.88899305555</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C47" s="2" t="n">
+        <v>45124.88957175926</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Оставить обращение</t>
+        </is>
+      </c>
+      <c r="C48" s="2" t="n">
+        <v>45124.88960648148</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C49" s="2" t="n">
+        <v>45124.89200231482</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Оставить обращение</t>
+        </is>
+      </c>
+      <c r="C50" s="2" t="n">
+        <v>45124.89201388889</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C51" s="2" t="n">
+        <v>45124.89356481482</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Оставить обращение</t>
+        </is>
+      </c>
+      <c r="C52" s="2" t="n">
+        <v>45124.89358796296</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C53" s="2" t="n">
+        <v>45124.89484953704</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Оставить обращение</t>
+        </is>
+      </c>
+      <c r="C54" s="2" t="n">
+        <v>45124.89487268519</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C55" s="2" t="n">
+        <v>45124.89611111111</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Оставить обращение</t>
+        </is>
+      </c>
+      <c r="C56" s="2" t="n">
+        <v>45124.89614583334</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C57" s="2" t="n">
+        <v>45124.89640046296</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Оставить обращение</t>
+        </is>
+      </c>
+      <c r="C58" s="2" t="n">
+        <v>45124.89642361111</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Learning.telecom.kz | Техническая поддержка</t>
+        </is>
+      </c>
+      <c r="C59" s="2" t="n">
+        <v>45124.89645833334</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C60" s="2" t="n">
+        <v>45124.89686342593</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Оставить обращение</t>
+        </is>
+      </c>
+      <c r="C61" s="2" t="n">
+        <v>45124.89689814814</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Learning.telecom.kz | Техническая поддержка</t>
+        </is>
+      </c>
+      <c r="C62" s="2" t="n">
+        <v>45124.8969212963</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C63" s="2" t="n">
+        <v>45124.89722222222</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Оставить обращение</t>
+        </is>
+      </c>
+      <c r="C64" s="2" t="n">
+        <v>45124.89724537037</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Learning.telecom.kz | Техническая поддержка</t>
+        </is>
+      </c>
+      <c r="C65" s="2" t="n">
+        <v>45124.89728009259</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C66" s="2" t="n">
+        <v>45124.899375</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Оставить обращение</t>
+        </is>
+      </c>
+      <c r="C67" s="2" t="n">
+        <v>45124.89939814815</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Learning.telecom.kz | Техническая поддержка</t>
+        </is>
+      </c>
+      <c r="C68" s="2" t="n">
+        <v>45124.89942129629</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C69" s="2" t="n">
+        <v>45124.89975694445</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Оставить обращение</t>
+        </is>
+      </c>
+      <c r="C70" s="2" t="n">
+        <v>45124.89979166666</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Learning.telecom.kz | Техническая поддержка</t>
+        </is>
+      </c>
+      <c r="C71" s="2" t="n">
+        <v>45124.89980324074</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C72" s="2" t="n">
+        <v>45124.90540509259</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Оставить обращение</t>
+        </is>
+      </c>
+      <c r="C73" s="2" t="n">
+        <v>45124.90543981481</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Learning.telecom.kz | Техническая поддержка</t>
+        </is>
+      </c>
+      <c r="C74" s="2" t="n">
+        <v>45124.90546296296</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C75" s="2" t="n">
+        <v>45124.91483796296</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Оставить обращение</t>
+        </is>
+      </c>
+      <c r="C76" s="2" t="n">
+        <v>45124.91488425926</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Learning.telecom.kz | Техническая поддержка</t>
+        </is>
+      </c>
+      <c r="C77" s="2" t="n">
+        <v>45124.91494212963</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C78" s="2" t="n">
+        <v>45124.91629629629</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Оставить обращение</t>
+        </is>
+      </c>
+      <c r="C79" s="2" t="n">
+        <v>45124.91631944444</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Learning.telecom.kz | Техническая поддержка</t>
+        </is>
+      </c>
+      <c r="C80" s="2" t="n">
+        <v>45124.91634259259</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C81" s="2" t="n">
+        <v>45124.92438657407</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="C82" s="2" t="n">
+        <v>45124.92444444444</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Өтінішті қалдыру</t>
+        </is>
+      </c>
+      <c r="C83" s="2" t="n">
+        <v>45124.92446759259</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Learning.telecom.kz | Техникалық қолдау</t>
+        </is>
+      </c>
+      <c r="C84" s="2" t="n">
+        <v>45124.92450231482</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>484489968</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="C85" s="2" t="n">
+        <v>45124.92577546297</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>484489968</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="C86" s="2" t="n">
+        <v>45124.92667824074</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>484489968</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Өтінішті қалдыру</t>
+        </is>
+      </c>
+      <c r="C87" s="2" t="n">
+        <v>45124.92793981481</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>484489968</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Комплаенс қызметіне хабарласыңыз</t>
+        </is>
+      </c>
+      <c r="C88" s="2" t="n">
+        <v>45124.92796296296</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>484489968</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Learning.telecom.kz | Техникалық қолдау</t>
+        </is>
+      </c>
+      <c r="C89" s="2" t="n">
+        <v>45124.92796296296</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="C90" s="2" t="n">
+        <v>45124.92893518518</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="C91" s="2" t="n">
+        <v>45124.93035879629</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C92" s="2" t="n">
+        <v>45124.93045138889</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C93" s="2" t="n">
+        <v>45124.9337037037</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Welcome курстар | Бейімделуі</t>
+        </is>
+      </c>
+      <c r="C94" s="2" t="n">
+        <v>45124.93372685185</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C95" s="2" t="n">
+        <v>45124.93378472222</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Білім базасы</t>
+        </is>
+      </c>
+      <c r="C96" s="2" t="n">
+        <v>45124.93381944444</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Нұсқаулық базасы</t>
+        </is>
+      </c>
+      <c r="C97" s="2" t="n">
+        <v>45124.93383101852</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C98" s="2" t="n">
+        <v>45124.93517361111</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Welcome курстар | Бейімделуі</t>
+        </is>
+      </c>
+      <c r="C99" s="2" t="n">
+        <v>45124.93521990741</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Айта бер!</t>
+        </is>
+      </c>
+      <c r="C100" s="2" t="n">
+        <v>45124.93527777777</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C101" s="2" t="n">
+        <v>45124.93721064815</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Жиі қойылатын сұрақтар</t>
+        </is>
+      </c>
+      <c r="C102" s="2" t="n">
+        <v>45124.93724537037</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>HR сұрақтары</t>
+        </is>
+      </c>
+      <c r="C103" s="2" t="n">
+        <v>45124.93725694445</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C104" s="2" t="n">
+        <v>45124.93732638889</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>БиОТ Картаны толтыру</t>
+        </is>
+      </c>
+      <c r="C105" s="2" t="n">
+        <v>45124.93734953704</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>қауіпті фактор/шарт</t>
+        </is>
+      </c>
+      <c r="C106" s="2" t="n">
+        <v>45124.93738425926</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Поведение при выполнении работ</t>
+        </is>
+      </c>
+      <c r="C107" s="2" t="n">
+        <v>45124.93740740741</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Предложения/Идеи</t>
+        </is>
+      </c>
+      <c r="C108" s="2" t="n">
+        <v>45124.93743055555</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C109" s="2" t="n">
+        <v>45124.93747685185</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>БиОТ Картаны толтыру</t>
+        </is>
+      </c>
+      <c r="C110" s="2" t="n">
+        <v>45124.93751157408</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C111" s="2" t="n">
+        <v>45124.93758101852</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Жиі қойылатын сұрақтар</t>
+        </is>
+      </c>
+      <c r="C112" s="2" t="n">
+        <v>45124.93761574074</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Демеу</t>
+        </is>
+      </c>
+      <c r="C113" s="2" t="n">
+        <v>45124.93762731482</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C114" s="2" t="n">
+        <v>45124.93766203704</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Білім базасы</t>
+        </is>
+      </c>
+      <c r="C115" s="2" t="n">
+        <v>45124.93767361111</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Нұсқаулық базасы</t>
+        </is>
+      </c>
+      <c r="C116" s="2" t="n">
+        <v>45124.93768518518</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C117" s="2" t="n">
+        <v>45124.94063657407</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Білім базасы</t>
+        </is>
+      </c>
+      <c r="C118" s="2" t="n">
+        <v>45124.94065972222</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Нұсқаулық базасы</t>
+        </is>
+      </c>
+      <c r="C119" s="2" t="n">
+        <v>45124.94068287037</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="C120" s="2" t="n">
+        <v>45124.94105324074</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Білім базасы</t>
+        </is>
+      </c>
+      <c r="C121" s="2" t="n">
+        <v>45124.94108796296</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Нұсқаулық базасы</t>
+        </is>
+      </c>
+      <c r="C122" s="2" t="n">
+        <v>45124.94112268519</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C123" s="2" t="n">
+        <v>45124.9412962963</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Білім базасы</t>
+        </is>
+      </c>
+      <c r="C124" s="2" t="n">
+        <v>45124.94131944444</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Нұсқаулық базасы</t>
+        </is>
+      </c>
+      <c r="C125" s="2" t="n">
+        <v>45124.94133101852</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C126" s="2" t="n">
+        <v>45124.94296296296</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Білім базасы</t>
+        </is>
+      </c>
+      <c r="C127" s="2" t="n">
+        <v>45124.94300925926</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Нұсқаулық базасы</t>
+        </is>
+      </c>
+      <c r="C128" s="2" t="n">
+        <v>45124.94303240741</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>portal.telecom.kz / нұсқаулар</t>
+        </is>
+      </c>
+      <c r="C129" s="2" t="n">
+        <v>45124.94307870371</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C130" s="2" t="n">
+        <v>45124.94319444444</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Өтінішті қалдыру</t>
+        </is>
+      </c>
+      <c r="C131" s="2" t="n">
+        <v>45124.94322916667</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Learning.telecom.kz | Техникалық қолдау</t>
+        </is>
+      </c>
+      <c r="C132" s="2" t="n">
+        <v>45124.94325231481</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C133" s="2" t="n">
+        <v>45124.94464120371</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Welcome курстар | Бейімделуі</t>
+        </is>
+      </c>
+      <c r="C134" s="2" t="n">
+        <v>45124.94467592592</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Айта бер!</t>
+        </is>
+      </c>
+      <c r="C135" s="2" t="n">
+        <v>45124.94472222222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docker, better kaz lang, new files
</commit_message>
<xml_diff>
--- a/output_file.xlsx
+++ b/output_file.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C135"/>
+  <dimension ref="A1:C155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2464,6 +2464,306 @@
         <v>45124.94472222222</v>
       </c>
     </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>187663574</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="C136" s="2" t="n">
+        <v>45124.94631944445</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>187663574</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="C137" s="2" t="n">
+        <v>45124.94635416667</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>187663574</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Welcome курс | Адаптация</t>
+        </is>
+      </c>
+      <c r="C138" s="2" t="n">
+        <v>45124.94658564815</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>187663574</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Рассказывай!</t>
+        </is>
+      </c>
+      <c r="C139" s="2" t="n">
+        <v>45124.94670138889</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>187663574</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Оставить обращение</t>
+        </is>
+      </c>
+      <c r="C140" s="2" t="n">
+        <v>45124.94673611111</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>187663574</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Learning.telecom.kz | Техническая поддержка</t>
+        </is>
+      </c>
+      <c r="C141" s="2" t="n">
+        <v>45124.94674768519</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>187663574</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Обучение | Корпоративный Университет</t>
+        </is>
+      </c>
+      <c r="C142" s="2" t="n">
+        <v>45124.9468287037</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>187663574</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Служба поддержки “Нысана"</t>
+        </is>
+      </c>
+      <c r="C143" s="2" t="n">
+        <v>45124.94685185186</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>187663574</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Обратиться в службу комплаенс</t>
+        </is>
+      </c>
+      <c r="C144" s="2" t="n">
+        <v>45124.946875</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>187663574</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="C145" s="2" t="n">
+        <v>45124.94689814815</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>187663574</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>База знаний</t>
+        </is>
+      </c>
+      <c r="C146" s="2" t="n">
+        <v>45124.94692129629</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>187663574</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>База инструкций</t>
+        </is>
+      </c>
+      <c r="C147" s="2" t="n">
+        <v>45124.94715277778</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>187663574</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>portal.telecom.kz | Инструкции</t>
+        </is>
+      </c>
+      <c r="C148" s="2" t="n">
+        <v>45124.9471875</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>187663574</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="C149" s="2" t="n">
+        <v>45124.94725694445</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>187663574</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Заполнить карточку БиОТ</t>
+        </is>
+      </c>
+      <c r="C150" s="2" t="n">
+        <v>45124.94729166666</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>187663574</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Опасный фактор/условие</t>
+        </is>
+      </c>
+      <c r="C151" s="2" t="n">
+        <v>45124.94730324074</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>187663574</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>menu</t>
+        </is>
+      </c>
+      <c r="C152" s="2" t="n">
+        <v>45124.94813657407</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>187663574</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Часто задаваемые вопросы</t>
+        </is>
+      </c>
+      <c r="C153" s="2" t="n">
+        <v>45124.9482175926</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>187663574</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Демеу</t>
+        </is>
+      </c>
+      <c r="C154" s="2" t="n">
+        <v>45124.94825231482</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>760906879</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>/start</t>
+        </is>
+      </c>
+      <c r="C155" s="2" t="n">
+        <v>45124.94930555556</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>